<commit_message>
added working multiple choice evaluator
</commit_message>
<xml_diff>
--- a/OCR/forms/out/sample.xlsx
+++ b/OCR/forms/out/sample.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,25 +449,25 @@
     <col customWidth="1" max="11" min="11" width="11"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row customHeight="1" ht="22.5" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>question1</t>
+          <t>leafwidth</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>question2</t>
+          <t>leafcolor</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>question3</t>
+          <t>pltheight</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>question4</t>
+          <t>lfprickle</t>
         </is>
       </c>
       <c r="E1" s="1" t="n"/>
@@ -478,18 +478,14 @@
       <c r="J1" s="1" t="n"/>
       <c r="K1" s="1" t="n"/>
     </row>
-    <row r="2">
+    <row customHeight="1" ht="22.5" r="2">
       <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C2" s="1" t="inlineStr"/>
       <c r="D2" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -503,18 +499,14 @@
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
     </row>
-    <row r="3">
+    <row customHeight="1" ht="22.5" r="3">
       <c r="A3" s="1" t="inlineStr"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C3" s="1" t="inlineStr"/>
       <c r="D3" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -528,18 +520,14 @@
       <c r="J3" s="1" t="n"/>
       <c r="K3" s="1" t="n"/>
     </row>
-    <row r="4">
+    <row customHeight="1" ht="22.5" r="4">
       <c r="A4" s="1" t="inlineStr"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C4" s="1" t="inlineStr"/>
       <c r="D4" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -553,18 +541,14 @@
       <c r="J4" s="1" t="n"/>
       <c r="K4" s="1" t="n"/>
     </row>
-    <row r="5">
+    <row customHeight="1" ht="22.5" r="5">
       <c r="A5" s="1" t="inlineStr"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -578,18 +562,14 @@
       <c r="J5" s="1" t="n"/>
       <c r="K5" s="1" t="n"/>
     </row>
-    <row r="6">
+    <row customHeight="1" ht="22.5" r="6">
       <c r="A6" s="1" t="inlineStr"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -603,18 +583,14 @@
       <c r="J6" s="1" t="n"/>
       <c r="K6" s="1" t="n"/>
     </row>
-    <row r="7">
+    <row customHeight="1" ht="22.5" r="7">
       <c r="A7" s="1" t="inlineStr"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -628,18 +604,14 @@
       <c r="J7" s="1" t="n"/>
       <c r="K7" s="1" t="n"/>
     </row>
-    <row r="8">
+    <row customHeight="1" ht="22.5" r="8">
       <c r="A8" s="1" t="inlineStr"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -653,18 +625,14 @@
       <c r="J8" s="1" t="n"/>
       <c r="K8" s="1" t="n"/>
     </row>
-    <row r="9">
+    <row customHeight="1" ht="22.5" r="9">
       <c r="A9" s="1" t="inlineStr"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -678,18 +646,14 @@
       <c r="J9" s="1" t="n"/>
       <c r="K9" s="1" t="n"/>
     </row>
-    <row r="10">
+    <row customHeight="1" ht="22.5" r="10">
       <c r="A10" s="1" t="inlineStr"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C10" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -703,18 +667,14 @@
       <c r="J10" s="1" t="n"/>
       <c r="K10" s="1" t="n"/>
     </row>
-    <row r="11">
+    <row customHeight="1" ht="22.5" r="11">
       <c r="A11" s="1" t="inlineStr"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C11" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -728,18 +688,14 @@
       <c r="J11" s="1" t="n"/>
       <c r="K11" s="1" t="n"/>
     </row>
-    <row r="12">
+    <row customHeight="1" ht="22.5" r="12">
       <c r="A12" s="1" t="inlineStr"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C12" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -753,18 +709,14 @@
       <c r="J12" s="1" t="n"/>
       <c r="K12" s="1" t="n"/>
     </row>
-    <row r="13">
+    <row customHeight="1" ht="22.5" r="13">
       <c r="A13" s="1" t="inlineStr"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C13" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -778,18 +730,14 @@
       <c r="J13" s="1" t="n"/>
       <c r="K13" s="1" t="n"/>
     </row>
-    <row r="14">
+    <row customHeight="1" ht="22.5" r="14">
       <c r="A14" s="1" t="inlineStr"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C14" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -803,18 +751,14 @@
       <c r="J14" s="1" t="n"/>
       <c r="K14" s="1" t="n"/>
     </row>
-    <row r="15">
+    <row customHeight="1" ht="22.5" r="15">
       <c r="A15" s="1" t="inlineStr"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C15" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -828,18 +772,14 @@
       <c r="J15" s="1" t="n"/>
       <c r="K15" s="1" t="n"/>
     </row>
-    <row r="16">
+    <row customHeight="1" ht="22.5" r="16">
       <c r="A16" s="1" t="inlineStr"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C16" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -853,18 +793,14 @@
       <c r="J16" s="1" t="n"/>
       <c r="K16" s="1" t="n"/>
     </row>
-    <row r="17">
+    <row customHeight="1" ht="22.5" r="17">
       <c r="A17" s="1" t="inlineStr"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C17" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -878,18 +814,14 @@
       <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
     </row>
-    <row r="18">
+    <row customHeight="1" ht="22.5" r="18">
       <c r="A18" s="1" t="inlineStr"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C18" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -903,18 +835,14 @@
       <c r="J18" s="1" t="n"/>
       <c r="K18" s="1" t="n"/>
     </row>
-    <row r="19">
+    <row customHeight="1" ht="22.5" r="19">
       <c r="A19" s="1" t="inlineStr"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C19" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -928,18 +856,14 @@
       <c r="J19" s="1" t="n"/>
       <c r="K19" s="1" t="n"/>
     </row>
-    <row r="20">
+    <row customHeight="1" ht="22.5" r="20">
       <c r="A20" s="1" t="inlineStr"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C20" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C20" s="1" t="inlineStr"/>
       <c r="D20" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -953,18 +877,14 @@
       <c r="J20" s="1" t="n"/>
       <c r="K20" s="1" t="n"/>
     </row>
-    <row r="21">
+    <row customHeight="1" ht="22.5" r="21">
       <c r="A21" s="1" t="inlineStr"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O O O O O O </t>
         </is>
       </c>
-      <c r="C21" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
+      <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">O O </t>
@@ -978,287 +898,12 @@
       <c r="J21" s="1" t="n"/>
       <c r="K21" s="1" t="n"/>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr"/>
-      <c r="B22" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C22" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D22" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E22" s="1" t="n"/>
-      <c r="F22" s="1" t="n"/>
-      <c r="G22" s="1" t="n"/>
-      <c r="H22" s="1" t="n"/>
-      <c r="I22" s="1" t="n"/>
-      <c r="J22" s="1" t="n"/>
-      <c r="K22" s="1" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr"/>
-      <c r="B23" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C23" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D23" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E23" s="1" t="n"/>
-      <c r="F23" s="1" t="n"/>
-      <c r="G23" s="1" t="n"/>
-      <c r="H23" s="1" t="n"/>
-      <c r="I23" s="1" t="n"/>
-      <c r="J23" s="1" t="n"/>
-      <c r="K23" s="1" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr"/>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C24" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D24" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E24" s="1" t="n"/>
-      <c r="F24" s="1" t="n"/>
-      <c r="G24" s="1" t="n"/>
-      <c r="H24" s="1" t="n"/>
-      <c r="I24" s="1" t="n"/>
-      <c r="J24" s="1" t="n"/>
-      <c r="K24" s="1" t="n"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr"/>
-      <c r="B25" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C25" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D25" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E25" s="1" t="n"/>
-      <c r="F25" s="1" t="n"/>
-      <c r="G25" s="1" t="n"/>
-      <c r="H25" s="1" t="n"/>
-      <c r="I25" s="1" t="n"/>
-      <c r="J25" s="1" t="n"/>
-      <c r="K25" s="1" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr"/>
-      <c r="B26" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C26" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D26" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E26" s="1" t="n"/>
-      <c r="F26" s="1" t="n"/>
-      <c r="G26" s="1" t="n"/>
-      <c r="H26" s="1" t="n"/>
-      <c r="I26" s="1" t="n"/>
-      <c r="J26" s="1" t="n"/>
-      <c r="K26" s="1" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr"/>
-      <c r="B27" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C27" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D27" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E27" s="1" t="n"/>
-      <c r="F27" s="1" t="n"/>
-      <c r="G27" s="1" t="n"/>
-      <c r="H27" s="1" t="n"/>
-      <c r="I27" s="1" t="n"/>
-      <c r="J27" s="1" t="n"/>
-      <c r="K27" s="1" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="inlineStr"/>
-      <c r="B28" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C28" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D28" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E28" s="1" t="n"/>
-      <c r="F28" s="1" t="n"/>
-      <c r="G28" s="1" t="n"/>
-      <c r="H28" s="1" t="n"/>
-      <c r="I28" s="1" t="n"/>
-      <c r="J28" s="1" t="n"/>
-      <c r="K28" s="1" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="inlineStr"/>
-      <c r="B29" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C29" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D29" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E29" s="1" t="n"/>
-      <c r="F29" s="1" t="n"/>
-      <c r="G29" s="1" t="n"/>
-      <c r="H29" s="1" t="n"/>
-      <c r="I29" s="1" t="n"/>
-      <c r="J29" s="1" t="n"/>
-      <c r="K29" s="1" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr"/>
-      <c r="B30" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C30" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D30" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E30" s="1" t="n"/>
-      <c r="F30" s="1" t="n"/>
-      <c r="G30" s="1" t="n"/>
-      <c r="H30" s="1" t="n"/>
-      <c r="I30" s="1" t="n"/>
-      <c r="J30" s="1" t="n"/>
-      <c r="K30" s="1" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="inlineStr"/>
-      <c r="B31" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C31" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D31" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E31" s="1" t="n"/>
-      <c r="F31" s="1" t="n"/>
-      <c r="G31" s="1" t="n"/>
-      <c r="H31" s="1" t="n"/>
-      <c r="I31" s="1" t="n"/>
-      <c r="J31" s="1" t="n"/>
-      <c r="K31" s="1" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="inlineStr"/>
-      <c r="B32" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O O O O O </t>
-        </is>
-      </c>
-      <c r="C32" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O O </t>
-        </is>
-      </c>
-      <c r="D32" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">O O </t>
-        </is>
-      </c>
-      <c r="E32" s="1" t="n"/>
-      <c r="F32" s="1" t="n"/>
-      <c r="G32" s="1" t="n"/>
-      <c r="H32" s="1" t="n"/>
-      <c r="I32" s="1" t="n"/>
-      <c r="J32" s="1" t="n"/>
-      <c r="K32" s="1" t="n"/>
-    </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <pageSetup fitToHeight="1" fitToWidth="1" orientation="landscape" paperSize="9"/>
   <headerFooter>
-    <oddHeader>&amp;LSample form</oddHeader>
+    <oddHeader>&amp;Lsample questionnaire 2&amp;R06/01/2021</oddHeader>
     <oddFooter/>
     <evenHeader/>
     <evenFooter/>

</xml_diff>